<commit_message>
Data files for q 1 and 2
</commit_message>
<xml_diff>
--- a/assignment_1/assignment_1.xlsx
+++ b/assignment_1/assignment_1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
   </bookViews>
   <sheets>
     <sheet name="problem1" sheetId="5" r:id="rId1"/>
@@ -18,6 +18,9 @@
     <sheet name="problem4_273_inf" sheetId="7" r:id="rId4"/>
     <sheet name="problem4_0_inf" sheetId="9" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="output_linearization_1_CV_31_output" localSheetId="1">problem2!$J$64:$Q$97</definedName>
+  </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -95,8 +98,27 @@
 </comments>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="output_linearization_1_CV_31_output" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="C:\Users\Alex\Documents\GitHub\CFD_course\assignment_1\problem_2\output_linearization_1_CV_31_output.txt" delimited="0">
+      <textFields count="8">
+        <textField/>
+        <textField position="2"/>
+        <textField position="7"/>
+        <textField position="17"/>
+        <textField position="29"/>
+        <textField position="40"/>
+        <textField position="51"/>
+        <textField position="61"/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="140">
   <si>
     <t>Trial</t>
   </si>
@@ -236,9 +258,6 @@
     <t>W/mK</t>
   </si>
   <si>
-    <t>Temperature distribution did not change over any of the iterations</t>
-  </si>
-  <si>
     <t>TINF</t>
   </si>
   <si>
@@ -287,9 +306,6 @@
     <t>X Pos</t>
   </si>
   <si>
-    <t>residuals did not reach criteriaf for IE = 65, stuck at 1.25E-5, converged to that value</t>
-  </si>
-  <si>
     <t>Y,Z</t>
   </si>
   <si>
@@ -501,6 +517,27 @@
   </si>
   <si>
     <t>residuals reached crit after 10 iterations, did not converge</t>
+  </si>
+  <si>
+    <t>residuals converged after 1st it. Didn't reach crit</t>
+  </si>
+  <si>
+    <t>residuals didn't reach crit, but converged after 1st it</t>
+  </si>
+  <si>
+    <t>reached crit after 1st it</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>I XP</t>
+  </si>
+  <si>
+    <t>T DE ATW</t>
+  </si>
+  <si>
+    <t>ATP BT</t>
   </si>
 </sst>
 </file>
@@ -510,7 +547,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000%"/>
     <numFmt numFmtId="165" formatCode="0.00000%"/>
-    <numFmt numFmtId="172" formatCode="0.00000"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -1737,6 +1774,35 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1755,15 +1821,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1771,26 +1828,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1859,22 +1896,11 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>problem2!$C$45</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Ts(x) [C]</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -1901,6 +1927,259 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
+              <c:f>problem2!$L$65:$L$97</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6129999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.8390000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0649999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.11291</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.14516999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.17743</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.20968999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.24195</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.27421000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.30647000000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.33872999999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.37098999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.40325</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.43551000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.46777000000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.50002999999999997</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.53229000000000004</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.56455</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.59680999999999995</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.62907000000000002</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.66132999999999997</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.69359000000000004</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.72585</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.75810999999999995</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.79037000000000002</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.82262999999999997</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.85489000000000004</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.88714999999999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.91940999999999995</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.95167000000000002</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.98392999999999997</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.0000599999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>problem2!$M$65:$M$97</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>373.14999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>366.38278000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>355.12061</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>345.75576999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>337.97626000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>331.52303999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>326.18124</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>321.77294999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>318.15134</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>315.19583</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>312.80795000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>310.90823</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>309.43340999999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>308.33434999999997</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>307.57445999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>307.12842000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>306.98138</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>307.12839000000002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>307.57443000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>308.33431999999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>309.43338</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>310.90820000000002</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>312.80788999999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>315.19574</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>318.15125</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>321.77283</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>326.18112000000002</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>331.52292</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>337.97613999999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>345.75565</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>355.12054000000001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>366.38272000000001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>373.14999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DB46-4949-9803-5D7A66860A1D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>series2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
               <c:f>problem2!$B$46:$B$77</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -2006,113 +2285,113 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>problem2!$C$46:$C$77</c:f>
+              <c:f>problem2!$D$46:$D$77</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>373.15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>82.954030027031223</c:v>
+                  <c:v>356.10403002703117</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>69.789109072715775</c:v>
+                  <c:v>342.93910907271572</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>59.623612450615759</c:v>
+                  <c:v>332.77361245061576</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>51.776780070864731</c:v>
+                  <c:v>324.92678007086471</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>45.723127491867075</c:v>
+                  <c:v>318.87312749186708</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>41.057255427498404</c:v>
+                  <c:v>314.20725542749835</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>37.466701082882665</c:v>
+                  <c:v>310.61670108288263</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>34.711013234712439</c:v>
+                  <c:v>307.8610132347124</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>32.605649762036585</c:v>
+                  <c:v>305.75564976203657</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>31.009619281930959</c:v>
+                  <c:v>304.15961928193093</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>29.816039278621162</c:v>
+                  <c:v>302.96603927862111</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>28.944978425530433</c:v>
+                  <c:v>302.09497842553043</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>28.338103766909224</c:v>
+                  <c:v>301.48810376690921</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>27.954774293026389</c:v>
+                  <c:v>301.10477429302637</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>27.769319304575259</c:v>
+                  <c:v>300.91931930457525</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>27.769319304575259</c:v>
+                  <c:v>300.91931930457525</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>27.954774293026389</c:v>
+                  <c:v>301.10477429302637</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>28.338103766909224</c:v>
+                  <c:v>301.48810376690921</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>28.944978425530433</c:v>
+                  <c:v>302.09497842553043</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>29.816039278621162</c:v>
+                  <c:v>302.96603927862111</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>31.009619281930956</c:v>
+                  <c:v>304.15961928193093</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>32.605649762036585</c:v>
+                  <c:v>305.75564976203657</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>34.711013234712439</c:v>
+                  <c:v>307.8610132347124</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>37.466701082882665</c:v>
+                  <c:v>310.61670108288263</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>41.057255427498404</c:v>
+                  <c:v>314.20725542749835</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>45.723127491867047</c:v>
+                  <c:v>318.87312749186702</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>51.776780070864731</c:v>
+                  <c:v>324.92678007086471</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>59.623612450615759</c:v>
+                  <c:v>332.77361245061576</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>69.78910907271576</c:v>
+                  <c:v>342.93910907271572</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>82.954030027031223</c:v>
+                  <c:v>356.10403002703117</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>100</c:v>
+                  <c:v>373.15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E3DB-4743-B940-CDA1A62E3B6C}"/>
+              <c16:uniqueId val="{00000001-DB46-4949-9803-5D7A66860A1D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2124,11 +2403,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="466715384"/>
-        <c:axId val="466714072"/>
+        <c:axId val="454081896"/>
+        <c:axId val="73910120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="466715384"/>
+        <c:axId val="454081896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2185,12 +2464,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="466714072"/>
+        <c:crossAx val="73910120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="466714072"/>
+        <c:axId val="73910120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2247,7 +2526,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="466715384"/>
+        <c:crossAx val="454081896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3942,22 +4221,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>74705</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>17930</xdr:rowOff>
+      <xdr:colOff>336176</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>144930</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1262530</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>141940</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>769470</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>19424</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD11FE37-9F1F-4590-AED0-6746823DC719}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F74A180-FDF9-415A-983A-3994068993B1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4017,6 +4296,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="output_linearization_1_CV_31_output" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4318,8 +4601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4468,7 +4751,7 @@
         <v>100</v>
       </c>
       <c r="G14" s="46">
-        <v>-1.9073486E-6</v>
+        <v>1.9073486E-6</v>
       </c>
       <c r="H14" s="42">
         <v>3.7500047699999999</v>
@@ -4476,9 +4759,7 @@
       <c r="I14" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="J14" s="10">
-        <v>6000.0073199999997</v>
-      </c>
+      <c r="J14" s="10"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="53">
@@ -4500,7 +4781,7 @@
         <v>100</v>
       </c>
       <c r="G15" s="48">
-        <v>-1.2715658000000001E-6</v>
+        <v>1.2715658000000001E-6</v>
       </c>
       <c r="H15" s="43">
         <v>3.7500092999999999</v>
@@ -4527,11 +4808,11 @@
         <v>0.125</v>
       </c>
       <c r="F16" s="2">
-        <f t="shared" ref="F16:F19" si="2">F15</f>
+        <f t="shared" ref="F16:F20" si="2">F15</f>
         <v>100</v>
       </c>
       <c r="G16" s="48">
-        <v>-3.2697409999999999E-6</v>
+        <v>5.4495676499999996E-6</v>
       </c>
       <c r="H16" s="43">
         <v>3.7500183599999999</v>
@@ -4541,7 +4822,7 @@
         <v>2.4159940083362396E-6</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17" s="53">
         <v>4</v>
       </c>
@@ -4562,7 +4843,7 @@
         <v>100</v>
       </c>
       <c r="G17" s="48">
-        <v>-6.1035157200000004E-6</v>
+        <v>1.6276042500000001E-5</v>
       </c>
       <c r="H17" s="43">
         <v>3.7500367200000002</v>
@@ -4571,8 +4852,11 @@
         <f t="shared" si="3"/>
         <v>4.8959760293888571E-6</v>
       </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J17" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B18" s="53">
         <v>5</v>
       </c>
@@ -4593,7 +4877,7 @@
         <v>100</v>
       </c>
       <c r="G18" s="49">
-        <v>-9.8443797499999997E-6</v>
+        <v>2.16576354E-5</v>
       </c>
       <c r="H18" s="56">
         <v>3.7501466300000001</v>
@@ -4602,8 +4886,11 @@
         <f t="shared" si="3"/>
         <v>2.9309046339134336E-5</v>
       </c>
-    </row>
-    <row r="19" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J18" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="54">
         <v>6</v>
       </c>
@@ -4624,33 +4911,49 @@
         <v>100</v>
       </c>
       <c r="G19" s="55">
-        <v>1.2500000000000001E-5</v>
+        <v>3.9721293400000003E-5</v>
       </c>
       <c r="H19" s="33">
-        <v>7.3851760000000004</v>
+        <v>3.7482149599999999</v>
       </c>
       <c r="I19" s="60">
         <f t="shared" si="3"/>
-        <v>0.9693032642832955</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="6"/>
-      <c r="C20" s="81" t="s">
-        <v>63</v>
-      </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+        <v>-5.1509185922158837E-4</v>
+      </c>
+      <c r="J19" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="54">
+        <v>7</v>
+      </c>
+      <c r="C20" s="50">
+        <v>2</v>
+      </c>
+      <c r="D20" s="18">
+        <f t="shared" ref="D20" si="5">C20-1</f>
+        <v>1</v>
+      </c>
+      <c r="E20" s="18">
+        <f t="shared" ref="E20" si="6">$D$4/D20</f>
+        <v>1</v>
+      </c>
+      <c r="F20" s="4">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="G20" s="55">
+        <v>0</v>
+      </c>
+      <c r="H20" s="33">
+        <v>3.7500002399999999</v>
+      </c>
+      <c r="I20" s="60"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B21" s="6"/>
-      <c r="C21" s="81" t="s">
-        <v>46</v>
-      </c>
+      <c r="C21" s="81"/>
       <c r="D21" s="6"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
@@ -4658,7 +4961,7 @@
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
@@ -4668,7 +4971,7 @@
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
@@ -4678,7 +4981,7 @@
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -4688,42 +4991,42 @@
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
@@ -4908,20 +5211,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W146"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="102" workbookViewId="0">
-      <selection activeCell="J46" sqref="J46"/>
+    <sheetView topLeftCell="A14" zoomScale="102" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="1.21875" customWidth="1"/>
     <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="3.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="44.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.21875" customWidth="1"/>
+    <col min="12" max="12" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.5546875" customWidth="1"/>
+    <col min="15" max="15" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.5546875" customWidth="1"/>
+    <col min="17" max="17" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="22.109375" customWidth="1"/>
     <col min="19" max="19" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13.5546875" bestFit="1" customWidth="1"/>
@@ -4932,132 +5240,132 @@
   <sheetData>
     <row r="1" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="111" t="s">
-        <v>110</v>
-      </c>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="113"/>
+      <c r="B2" s="132" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="133"/>
+      <c r="D2" s="133"/>
+      <c r="E2" s="134"/>
       <c r="G2" s="27" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B3" s="137" t="s">
+      <c r="B3" s="125" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="125" t="s">
+      <c r="C3" s="113" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="125">
+      <c r="D3" s="113">
         <v>1</v>
       </c>
-      <c r="E3" s="126" t="s">
+      <c r="E3" s="114" t="s">
         <v>19</v>
       </c>
       <c r="M3" s="27"/>
     </row>
     <row r="4" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B4" s="127" t="s">
+      <c r="B4" s="115" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="123"/>
-      <c r="D4" s="123">
+      <c r="C4" s="111"/>
+      <c r="D4" s="111">
         <v>7800</v>
       </c>
-      <c r="E4" s="128" t="s">
+      <c r="E4" s="116" t="s">
         <v>44</v>
       </c>
       <c r="M4" s="27"/>
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B5" s="127" t="s">
+      <c r="B5" s="115" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="123"/>
-      <c r="D5" s="123">
+      <c r="C5" s="111"/>
+      <c r="D5" s="111">
         <v>60</v>
       </c>
-      <c r="E5" s="128" t="s">
+      <c r="E5" s="116" t="s">
         <v>45</v>
       </c>
       <c r="M5" s="27"/>
     </row>
     <row r="6" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B6" s="127" t="s">
+      <c r="B6" s="115" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="123"/>
-      <c r="D6" s="123">
+      <c r="C6" s="111"/>
+      <c r="D6" s="111">
         <v>430</v>
       </c>
-      <c r="E6" s="128" t="s">
+      <c r="E6" s="116" t="s">
         <v>43</v>
       </c>
       <c r="M6" s="27"/>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B7" s="127" t="s">
+      <c r="B7" s="115" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="123"/>
-      <c r="D7" s="123">
+      <c r="C7" s="111"/>
+      <c r="D7" s="111">
         <v>12</v>
       </c>
-      <c r="E7" s="128" t="s">
+      <c r="E7" s="116" t="s">
         <v>42</v>
       </c>
       <c r="M7" s="27"/>
     </row>
     <row r="8" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B8" s="127" t="s">
+      <c r="B8" s="115" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="123"/>
-      <c r="D8" s="123">
+      <c r="C8" s="111"/>
+      <c r="D8" s="111">
         <v>100</v>
       </c>
-      <c r="E8" s="128" t="s">
+      <c r="E8" s="116" t="s">
         <v>41</v>
       </c>
       <c r="M8" s="27"/>
     </row>
     <row r="9" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B9" s="127" t="s">
+      <c r="B9" s="115" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="123"/>
-      <c r="D9" s="123">
+      <c r="C9" s="111"/>
+      <c r="D9" s="111">
         <v>100</v>
       </c>
-      <c r="E9" s="128" t="s">
+      <c r="E9" s="116" t="s">
         <v>41</v>
       </c>
       <c r="M9" s="27"/>
     </row>
     <row r="10" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B10" s="138" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="123"/>
-      <c r="D10" s="123">
+      <c r="B10" s="126" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="111"/>
+      <c r="D10" s="111">
         <v>25</v>
       </c>
-      <c r="E10" s="128" t="s">
+      <c r="E10" s="116" t="s">
         <v>41</v>
       </c>
       <c r="M10" s="27"/>
     </row>
     <row r="11" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="139" t="s">
-        <v>109</v>
-      </c>
-      <c r="C11" s="129"/>
-      <c r="D11" s="129">
+      <c r="B11" s="127" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" s="117"/>
+      <c r="D11" s="117">
         <f>0.0125</f>
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="E11" s="130" t="s">
+      <c r="E11" s="118" t="s">
         <v>19</v>
       </c>
       <c r="M11" s="27"/>
@@ -5068,12 +5376,12 @@
     </row>
     <row r="13" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="45"/>
-      <c r="G13" s="111" t="s">
+      <c r="G13" s="132" t="s">
         <v>32</v>
       </c>
-      <c r="H13" s="112"/>
-      <c r="I13" s="112"/>
-      <c r="J13" s="113"/>
+      <c r="H13" s="133"/>
+      <c r="I13" s="133"/>
+      <c r="J13" s="134"/>
       <c r="M13" s="45" t="s">
         <v>17</v>
       </c>
@@ -5117,16 +5425,16 @@
       </c>
       <c r="K14" s="80"/>
       <c r="M14" s="45"/>
-      <c r="R14" s="111" t="s">
+      <c r="R14" s="132" t="s">
         <v>22</v>
       </c>
-      <c r="S14" s="112"/>
-      <c r="T14" s="113"/>
-      <c r="U14" s="111" t="s">
+      <c r="S14" s="133"/>
+      <c r="T14" s="134"/>
+      <c r="U14" s="132" t="s">
         <v>23</v>
       </c>
-      <c r="V14" s="112"/>
-      <c r="W14" s="113"/>
+      <c r="V14" s="133"/>
+      <c r="W14" s="134"/>
     </row>
     <row r="15" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="19">
@@ -5541,11 +5849,11 @@
       <c r="O21" s="6"/>
       <c r="P21" s="6"/>
       <c r="Q21" s="6"/>
-      <c r="R21" s="111" t="s">
+      <c r="R21" s="132" t="s">
         <v>24</v>
       </c>
-      <c r="S21" s="112"/>
-      <c r="T21" s="113"/>
+      <c r="S21" s="133"/>
+      <c r="T21" s="134"/>
     </row>
     <row r="22" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="6"/>
@@ -5580,11 +5888,11 @@
     </row>
     <row r="23" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="45"/>
-      <c r="G23" s="111" t="s">
-        <v>48</v>
-      </c>
-      <c r="H23" s="112"/>
-      <c r="I23" s="113"/>
+      <c r="G23" s="132" t="s">
+        <v>47</v>
+      </c>
+      <c r="H23" s="133"/>
+      <c r="I23" s="134"/>
       <c r="J23" s="6"/>
       <c r="M23" s="19">
         <v>1</v>
@@ -5628,13 +5936,13 @@
         <v>8</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H24" s="8" t="s">
         <v>20</v>
       </c>
       <c r="I24" s="71" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M24" s="20">
         <v>2</v>
@@ -5690,7 +5998,7 @@
       </c>
       <c r="I25" s="72"/>
       <c r="J25" t="s">
-        <v>97</v>
+        <v>134</v>
       </c>
       <c r="M25" s="20">
         <v>3</v>
@@ -5748,6 +6056,9 @@
         <f>(G26-G25)/G25</f>
         <v>0.28047145154102143</v>
       </c>
+      <c r="J26" t="s">
+        <v>135</v>
+      </c>
       <c r="M26" s="20">
         <v>4</v>
       </c>
@@ -5805,7 +6116,7 @@
         <v>6.0765911529266935E-2</v>
       </c>
       <c r="J27" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="M27" s="64">
         <v>5</v>
@@ -5864,7 +6175,7 @@
         <v>1.3590426064108206E-2</v>
       </c>
       <c r="J28" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="N28" s="6"/>
       <c r="O28" s="6"/>
@@ -5903,7 +6214,7 @@
         <v>3.1413368037167518E-3</v>
       </c>
       <c r="J29" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="N29" s="6"/>
       <c r="O29" s="6"/>
@@ -5944,20 +6255,20 @@
       <c r="O30" s="6"/>
       <c r="P30" s="6"/>
       <c r="Q30" s="6"/>
-      <c r="R30" s="111" t="s">
+      <c r="R30" s="132" t="s">
         <v>28</v>
       </c>
-      <c r="S30" s="112"/>
-      <c r="T30" s="112"/>
-      <c r="U30" s="113"/>
+      <c r="S30" s="133"/>
+      <c r="T30" s="133"/>
+      <c r="U30" s="134"/>
     </row>
     <row r="31" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="45"/>
-      <c r="G31" s="111" t="s">
-        <v>50</v>
-      </c>
-      <c r="H31" s="112"/>
-      <c r="I31" s="113"/>
+      <c r="G31" s="132" t="s">
+        <v>49</v>
+      </c>
+      <c r="H31" s="133"/>
+      <c r="I31" s="134"/>
       <c r="M31" s="11" t="s">
         <v>0</v>
       </c>
@@ -6009,13 +6320,13 @@
         <v>8</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H32" s="8" t="s">
         <v>20</v>
       </c>
       <c r="I32" s="71" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M32" s="19">
         <v>1</v>
@@ -6084,7 +6395,7 @@
       <c r="I33" s="72"/>
       <c r="J33" t="str">
         <f>J25</f>
-        <v>residuals didn't reach crit, but converged</v>
+        <v>residuals didn't reach crit, but converged after 1st it</v>
       </c>
       <c r="M33" s="20">
         <v>2</v>
@@ -6154,9 +6465,9 @@
         <f>(G34-G33)/G33</f>
         <v>6.2723862288071664E-3</v>
       </c>
-      <c r="J34">
+      <c r="J34" t="str">
         <f t="shared" ref="J34:J38" si="19">J26</f>
-        <v>0</v>
+        <v>reached crit after 1st it</v>
       </c>
       <c r="M34" s="20">
         <v>3</v>
@@ -6457,35 +6768,35 @@
       <c r="T39" s="7"/>
     </row>
     <row r="40" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="124" t="s">
-        <v>107</v>
-      </c>
-      <c r="C40" s="126">
+      <c r="B40" s="112" t="s">
+        <v>105</v>
+      </c>
+      <c r="C40" s="114">
         <f>2*D11+2*D11</f>
         <v>0.05</v>
       </c>
-      <c r="D40" s="136"/>
+      <c r="D40" s="124"/>
       <c r="M40" s="6"/>
       <c r="N40" s="6"/>
       <c r="O40" s="6"/>
       <c r="P40" s="6"/>
       <c r="Q40" s="6"/>
-      <c r="R40" s="111" t="s">
+      <c r="R40" s="132" t="s">
         <v>29</v>
       </c>
-      <c r="S40" s="112"/>
-      <c r="T40" s="112"/>
-      <c r="U40" s="113"/>
+      <c r="S40" s="133"/>
+      <c r="T40" s="133"/>
+      <c r="U40" s="134"/>
     </row>
     <row r="41" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="127" t="s">
-        <v>108</v>
-      </c>
-      <c r="C41" s="128">
+      <c r="B41" s="115" t="s">
+        <v>106</v>
+      </c>
+      <c r="C41" s="116">
         <f>D11*D11</f>
         <v>1.5625000000000003E-4</v>
       </c>
-      <c r="D41" s="133"/>
+      <c r="D41" s="121"/>
       <c r="M41" s="11" t="s">
         <v>0</v>
       </c>
@@ -6521,14 +6832,14 @@
       </c>
     </row>
     <row r="42" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="134" t="s">
+      <c r="B42" s="122" t="s">
         <v>19</v>
       </c>
-      <c r="C42" s="135">
+      <c r="C42" s="123">
         <f>SQRT(D7*C40/D5/C41)</f>
         <v>8</v>
       </c>
-      <c r="D42" s="133"/>
+      <c r="D42" s="121"/>
       <c r="M42" s="19">
         <v>1</v>
       </c>
@@ -6565,9 +6876,9 @@
       </c>
     </row>
     <row r="43" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="131"/>
-      <c r="C43" s="132"/>
-      <c r="D43" s="133"/>
+      <c r="B43" s="119"/>
+      <c r="C43" s="120"/>
+      <c r="D43" s="121"/>
       <c r="M43" s="20">
         <v>2</v>
       </c>
@@ -6608,11 +6919,11 @@
       </c>
     </row>
     <row r="44" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="117" t="s">
-        <v>103</v>
-      </c>
-      <c r="C44" s="118"/>
-      <c r="D44" s="119"/>
+      <c r="B44" s="129" t="s">
+        <v>101</v>
+      </c>
+      <c r="C44" s="130"/>
+      <c r="D44" s="131"/>
       <c r="M44" s="20">
         <v>3</v>
       </c>
@@ -6654,13 +6965,13 @@
     </row>
     <row r="45" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B45" s="12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D45" s="14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="M45" s="20">
         <v>4</v>
@@ -7137,11 +7448,22 @@
         <f t="shared" si="29"/>
         <v>301.48810376690921</v>
       </c>
-      <c r="M64" s="6"/>
+      <c r="J64" t="s">
+        <v>136</v>
+      </c>
+      <c r="K64" t="s">
+        <v>137</v>
+      </c>
+      <c r="L64" t="s">
+        <v>138</v>
+      </c>
+      <c r="M64" s="6" t="s">
+        <v>139</v>
+      </c>
       <c r="N64" s="6"/>
       <c r="O64" s="6"/>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>19</v>
       </c>
@@ -7157,11 +7479,29 @@
         <f t="shared" si="29"/>
         <v>302.09497842553043</v>
       </c>
-      <c r="M65" s="6"/>
-      <c r="N65" s="6"/>
-      <c r="O65" s="6"/>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K65">
+        <v>1</v>
+      </c>
+      <c r="L65">
+        <v>0</v>
+      </c>
+      <c r="M65" s="6">
+        <v>373.14999</v>
+      </c>
+      <c r="N65" s="6">
+        <v>2.3248600000000001</v>
+      </c>
+      <c r="O65" s="6">
+        <v>0</v>
+      </c>
+      <c r="P65">
+        <v>1</v>
+      </c>
+      <c r="Q65">
+        <v>373.14999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>20</v>
       </c>
@@ -7177,11 +7517,29 @@
         <f t="shared" si="29"/>
         <v>302.96603927862111</v>
       </c>
-      <c r="M66" s="6"/>
-      <c r="N66" s="6"/>
-      <c r="O66" s="6"/>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K66">
+        <v>2</v>
+      </c>
+      <c r="L66">
+        <v>1.6129999999999999E-2</v>
+      </c>
+      <c r="M66" s="6">
+        <v>366.38278000000003</v>
+      </c>
+      <c r="N66" s="6">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="O66" s="6">
+        <v>2.3248600000000001</v>
+      </c>
+      <c r="P66">
+        <v>3.5259999999999998</v>
+      </c>
+      <c r="Q66">
+        <v>11.541980000000001</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>21</v>
       </c>
@@ -7197,11 +7555,29 @@
         <f t="shared" si="29"/>
         <v>304.15961928193093</v>
       </c>
-      <c r="M67" s="6"/>
-      <c r="N67" s="6"/>
-      <c r="O67" s="6"/>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K67">
+        <v>3</v>
+      </c>
+      <c r="L67">
+        <v>4.8390000000000002E-2</v>
+      </c>
+      <c r="M67" s="6">
+        <v>355.12061</v>
+      </c>
+      <c r="N67" s="6">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="O67" s="6">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="P67">
+        <v>2.3635700000000002</v>
+      </c>
+      <c r="Q67">
+        <v>11.541980000000001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>22</v>
       </c>
@@ -7217,11 +7593,29 @@
         <f t="shared" si="29"/>
         <v>305.75564976203657</v>
       </c>
-      <c r="M68" s="6"/>
-      <c r="N68" s="6"/>
-      <c r="O68" s="6"/>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K68">
+        <v>4</v>
+      </c>
+      <c r="L68">
+        <v>8.0649999999999999E-2</v>
+      </c>
+      <c r="M68" s="6">
+        <v>345.75576999999998</v>
+      </c>
+      <c r="N68" s="6">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="O68" s="6">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="P68">
+        <v>2.3635700000000002</v>
+      </c>
+      <c r="Q68">
+        <v>11.541980000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>23</v>
       </c>
@@ -7237,11 +7631,29 @@
         <f t="shared" si="29"/>
         <v>307.8610132347124</v>
       </c>
-      <c r="M69" s="6"/>
-      <c r="N69" s="6"/>
-      <c r="O69" s="6"/>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K69">
+        <v>5</v>
+      </c>
+      <c r="L69">
+        <v>0.11291</v>
+      </c>
+      <c r="M69" s="6">
+        <v>337.97626000000002</v>
+      </c>
+      <c r="N69" s="6">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="O69" s="6">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="P69">
+        <v>2.3635700000000002</v>
+      </c>
+      <c r="Q69">
+        <v>11.541980000000001</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>24</v>
       </c>
@@ -7257,11 +7669,29 @@
         <f t="shared" si="29"/>
         <v>310.61670108288263</v>
       </c>
-      <c r="M70" s="6"/>
-      <c r="N70" s="6"/>
-      <c r="O70" s="6"/>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K70">
+        <v>6</v>
+      </c>
+      <c r="L70">
+        <v>0.14516999999999999</v>
+      </c>
+      <c r="M70" s="6">
+        <v>331.52303999999998</v>
+      </c>
+      <c r="N70" s="6">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="O70" s="6">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="P70">
+        <v>2.3635700000000002</v>
+      </c>
+      <c r="Q70">
+        <v>11.541980000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>25</v>
       </c>
@@ -7277,11 +7707,29 @@
         <f t="shared" si="29"/>
         <v>314.20725542749835</v>
       </c>
-      <c r="M71" s="6"/>
-      <c r="N71" s="6"/>
-      <c r="O71" s="6"/>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K71">
+        <v>7</v>
+      </c>
+      <c r="L71">
+        <v>0.17743</v>
+      </c>
+      <c r="M71" s="6">
+        <v>326.18124</v>
+      </c>
+      <c r="N71" s="6">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="O71" s="6">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="P71">
+        <v>2.3635700000000002</v>
+      </c>
+      <c r="Q71">
+        <v>11.541980000000001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>26</v>
       </c>
@@ -7297,11 +7745,29 @@
         <f t="shared" si="29"/>
         <v>318.87312749186702</v>
       </c>
-      <c r="M72" s="6"/>
-      <c r="N72" s="6"/>
-      <c r="O72" s="6"/>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K72">
+        <v>8</v>
+      </c>
+      <c r="L72">
+        <v>0.20968999999999999</v>
+      </c>
+      <c r="M72" s="6">
+        <v>321.77294999999998</v>
+      </c>
+      <c r="N72" s="6">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="O72" s="6">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="P72">
+        <v>2.3635700000000002</v>
+      </c>
+      <c r="Q72">
+        <v>11.541980000000001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>27</v>
       </c>
@@ -7317,11 +7783,29 @@
         <f t="shared" si="29"/>
         <v>324.92678007086471</v>
       </c>
-      <c r="M73" s="6"/>
-      <c r="N73" s="6"/>
-      <c r="O73" s="6"/>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K73">
+        <v>9</v>
+      </c>
+      <c r="L73">
+        <v>0.24195</v>
+      </c>
+      <c r="M73" s="6">
+        <v>318.15134</v>
+      </c>
+      <c r="N73" s="6">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="O73" s="6">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="P73">
+        <v>2.3635700000000002</v>
+      </c>
+      <c r="Q73">
+        <v>11.541980000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>28</v>
       </c>
@@ -7337,11 +7821,29 @@
         <f t="shared" si="29"/>
         <v>332.77361245061576</v>
       </c>
-      <c r="M74" s="6"/>
-      <c r="N74" s="6"/>
-      <c r="O74" s="6"/>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K74">
+        <v>10</v>
+      </c>
+      <c r="L74">
+        <v>0.27421000000000001</v>
+      </c>
+      <c r="M74" s="6">
+        <v>315.19583</v>
+      </c>
+      <c r="N74" s="6">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="O74" s="6">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="P74">
+        <v>2.3635700000000002</v>
+      </c>
+      <c r="Q74">
+        <v>11.541980000000001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>29</v>
       </c>
@@ -7357,11 +7859,29 @@
         <f t="shared" si="29"/>
         <v>342.93910907271572</v>
       </c>
-      <c r="M75" s="6"/>
-      <c r="N75" s="6"/>
-      <c r="O75" s="6"/>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K75">
+        <v>11</v>
+      </c>
+      <c r="L75">
+        <v>0.30647000000000002</v>
+      </c>
+      <c r="M75" s="6">
+        <v>312.80795000000001</v>
+      </c>
+      <c r="N75" s="6">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="O75" s="6">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="P75">
+        <v>2.3635700000000002</v>
+      </c>
+      <c r="Q75">
+        <v>11.541980000000001</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>30</v>
       </c>
@@ -7377,11 +7897,29 @@
         <f t="shared" si="29"/>
         <v>356.10403002703117</v>
       </c>
-      <c r="M76" s="6"/>
-      <c r="N76" s="6"/>
-      <c r="O76" s="6"/>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K76">
+        <v>12</v>
+      </c>
+      <c r="L76">
+        <v>0.33872999999999998</v>
+      </c>
+      <c r="M76" s="6">
+        <v>310.90823</v>
+      </c>
+      <c r="N76" s="6">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="O76" s="6">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="P76">
+        <v>2.3635700000000002</v>
+      </c>
+      <c r="Q76">
+        <v>11.541980000000001</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>31</v>
       </c>
@@ -7397,11 +7935,29 @@
         <f t="shared" si="29"/>
         <v>373.15</v>
       </c>
-      <c r="M77" s="6"/>
-      <c r="N77" s="6"/>
-      <c r="O77" s="6"/>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K77">
+        <v>13</v>
+      </c>
+      <c r="L77">
+        <v>0.37098999999999999</v>
+      </c>
+      <c r="M77" s="6">
+        <v>309.43340999999998</v>
+      </c>
+      <c r="N77" s="6">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="O77" s="6">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="P77">
+        <v>2.3635700000000002</v>
+      </c>
+      <c r="Q77">
+        <v>11.541980000000001</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>32</v>
       </c>
@@ -7417,11 +7973,29 @@
         <f t="shared" si="29"/>
         <v>395.2185486661715</v>
       </c>
-      <c r="M78" s="6"/>
-      <c r="N78" s="6"/>
-      <c r="O78" s="6"/>
-    </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K78">
+        <v>14</v>
+      </c>
+      <c r="L78">
+        <v>0.40325</v>
+      </c>
+      <c r="M78" s="6">
+        <v>308.33434999999997</v>
+      </c>
+      <c r="N78" s="6">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="O78" s="6">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="P78">
+        <v>2.3635700000000002</v>
+      </c>
+      <c r="Q78">
+        <v>11.541980000000001</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>33</v>
       </c>
@@ -7436,11 +8010,29 @@
         <f t="shared" si="29"/>
         <v>303.85275011525772</v>
       </c>
-      <c r="M79" s="6"/>
-      <c r="N79" s="6"/>
-      <c r="O79" s="6"/>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K79">
+        <v>15</v>
+      </c>
+      <c r="L79">
+        <v>0.43551000000000001</v>
+      </c>
+      <c r="M79" s="6">
+        <v>307.57445999999999</v>
+      </c>
+      <c r="N79" s="6">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="O79" s="6">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="P79">
+        <v>2.3635700000000002</v>
+      </c>
+      <c r="Q79">
+        <v>11.541980000000001</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>34</v>
       </c>
@@ -7455,11 +8047,29 @@
         <f t="shared" si="29"/>
         <v>303.47075397732101</v>
       </c>
-      <c r="M80" s="6"/>
-      <c r="N80" s="6"/>
-      <c r="O80" s="6"/>
-    </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K80">
+        <v>16</v>
+      </c>
+      <c r="L80">
+        <v>0.46777000000000002</v>
+      </c>
+      <c r="M80" s="6">
+        <v>307.12842000000001</v>
+      </c>
+      <c r="N80" s="6">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="O80" s="6">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="P80">
+        <v>2.3635700000000002</v>
+      </c>
+      <c r="Q80">
+        <v>11.541980000000001</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>35</v>
       </c>
@@ -7474,11 +8084,29 @@
         <f t="shared" si="29"/>
         <v>303.1228288302209</v>
       </c>
-      <c r="M81" s="6"/>
-      <c r="N81" s="6"/>
-      <c r="O81" s="6"/>
-    </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K81">
+        <v>17</v>
+      </c>
+      <c r="L81">
+        <v>0.50002999999999997</v>
+      </c>
+      <c r="M81" s="6">
+        <v>306.98138</v>
+      </c>
+      <c r="N81" s="6">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="O81" s="6">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="P81">
+        <v>2.3635700000000002</v>
+      </c>
+      <c r="Q81">
+        <v>11.541980000000001</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>36</v>
       </c>
@@ -7493,11 +8121,29 @@
         <f t="shared" si="29"/>
         <v>302.8067467651781</v>
       </c>
-      <c r="M82" s="6"/>
-      <c r="N82" s="6"/>
-      <c r="O82" s="6"/>
-    </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K82">
+        <v>18</v>
+      </c>
+      <c r="L82">
+        <v>0.53229000000000004</v>
+      </c>
+      <c r="M82" s="6">
+        <v>307.12839000000002</v>
+      </c>
+      <c r="N82" s="6">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="O82" s="6">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="P82">
+        <v>2.3635700000000002</v>
+      </c>
+      <c r="Q82">
+        <v>11.541980000000001</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>37</v>
       </c>
@@ -7512,8 +8158,29 @@
         <f t="shared" si="29"/>
         <v>302.5204837778528</v>
       </c>
-    </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K83">
+        <v>19</v>
+      </c>
+      <c r="L83">
+        <v>0.56455</v>
+      </c>
+      <c r="M83">
+        <v>307.57443000000001</v>
+      </c>
+      <c r="N83">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="O83">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="P83">
+        <v>2.3635700000000002</v>
+      </c>
+      <c r="Q83">
+        <v>11.541980000000001</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>38</v>
       </c>
@@ -7528,8 +8195,29 @@
         <f t="shared" si="29"/>
         <v>302.26220680780654</v>
       </c>
-    </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K84">
+        <v>20</v>
+      </c>
+      <c r="L84">
+        <v>0.59680999999999995</v>
+      </c>
+      <c r="M84">
+        <v>308.33431999999999</v>
+      </c>
+      <c r="N84">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="O84">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="P84">
+        <v>2.3635700000000002</v>
+      </c>
+      <c r="Q84">
+        <v>11.541980000000001</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>39</v>
       </c>
@@ -7544,8 +8232,29 @@
         <f t="shared" si="29"/>
         <v>302.03026200065756</v>
       </c>
-    </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K85">
+        <v>21</v>
+      </c>
+      <c r="L85">
+        <v>0.62907000000000002</v>
+      </c>
+      <c r="M85">
+        <v>309.43338</v>
+      </c>
+      <c r="N85">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="O85">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="P85">
+        <v>2.3635700000000002</v>
+      </c>
+      <c r="Q85">
+        <v>11.541980000000001</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>40</v>
       </c>
@@ -7560,8 +8269,29 @@
         <f t="shared" si="29"/>
         <v>301.82316411776628</v>
       </c>
-    </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K86">
+        <v>22</v>
+      </c>
+      <c r="L86">
+        <v>0.66132999999999997</v>
+      </c>
+      <c r="M86">
+        <v>310.90820000000002</v>
+      </c>
+      <c r="N86">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="O86">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="P86">
+        <v>2.3635700000000002</v>
+      </c>
+      <c r="Q86">
+        <v>11.541980000000001</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>41</v>
       </c>
@@ -7576,8 +8306,29 @@
         <f t="shared" si="29"/>
         <v>301.63958702563724</v>
       </c>
-    </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K87">
+        <v>23</v>
+      </c>
+      <c r="L87">
+        <v>0.69359000000000004</v>
+      </c>
+      <c r="M87">
+        <v>312.80788999999999</v>
+      </c>
+      <c r="N87">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="O87">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="P87">
+        <v>2.3635700000000002</v>
+      </c>
+      <c r="Q87">
+        <v>11.541980000000001</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>42</v>
       </c>
@@ -7592,8 +8343,29 @@
         <f t="shared" si="29"/>
         <v>301.4783552041373</v>
       </c>
-    </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K88">
+        <v>24</v>
+      </c>
+      <c r="L88">
+        <v>0.72585</v>
+      </c>
+      <c r="M88">
+        <v>315.19574</v>
+      </c>
+      <c r="N88">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="O88">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="P88">
+        <v>2.3635700000000002</v>
+      </c>
+      <c r="Q88">
+        <v>11.541980000000001</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>43</v>
       </c>
@@ -7608,8 +8380,29 @@
         <f t="shared" si="29"/>
         <v>301.33843621915355</v>
       </c>
-    </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K89">
+        <v>25</v>
+      </c>
+      <c r="L89">
+        <v>0.75810999999999995</v>
+      </c>
+      <c r="M89">
+        <v>318.15125</v>
+      </c>
+      <c r="N89">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="O89">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="P89">
+        <v>2.3635700000000002</v>
+      </c>
+      <c r="Q89">
+        <v>11.541980000000001</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>44</v>
       </c>
@@ -7624,8 +8417,29 @@
         <f t="shared" si="29"/>
         <v>301.21893411149006</v>
       </c>
-    </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K90">
+        <v>26</v>
+      </c>
+      <c r="L90">
+        <v>0.79037000000000002</v>
+      </c>
+      <c r="M90">
+        <v>321.77283</v>
+      </c>
+      <c r="N90">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="O90">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="P90">
+        <v>2.3635700000000002</v>
+      </c>
+      <c r="Q90">
+        <v>11.541980000000001</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>45</v>
       </c>
@@ -7640,8 +8454,29 @@
         <f t="shared" si="29"/>
         <v>301.11908365967014</v>
       </c>
-    </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K91">
+        <v>27</v>
+      </c>
+      <c r="L91">
+        <v>0.82262999999999997</v>
+      </c>
+      <c r="M91">
+        <v>326.18112000000002</v>
+      </c>
+      <c r="N91">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="O91">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="P91">
+        <v>2.3635700000000002</v>
+      </c>
+      <c r="Q91">
+        <v>11.541980000000001</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>46</v>
       </c>
@@ -7656,8 +8491,29 @@
         <f t="shared" si="29"/>
         <v>301.03824547990661</v>
       </c>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K92">
+        <v>28</v>
+      </c>
+      <c r="L92">
+        <v>0.85489000000000004</v>
+      </c>
+      <c r="M92">
+        <v>331.52292</v>
+      </c>
+      <c r="N92">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="O92">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="P92">
+        <v>2.3635700000000002</v>
+      </c>
+      <c r="Q92">
+        <v>11.541980000000001</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>47</v>
       </c>
@@ -7672,8 +8528,29 @@
         <f t="shared" si="29"/>
         <v>300.97590193186244</v>
       </c>
-    </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K93">
+        <v>29</v>
+      </c>
+      <c r="L93">
+        <v>0.88714999999999999</v>
+      </c>
+      <c r="M93">
+        <v>337.97613999999999</v>
+      </c>
+      <c r="N93">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="O93">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="P93">
+        <v>2.3635700000000002</v>
+      </c>
+      <c r="Q93">
+        <v>11.541980000000001</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>48</v>
       </c>
@@ -7688,8 +8565,29 @@
         <f t="shared" si="29"/>
         <v>300.93165380398545</v>
       </c>
-    </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K94">
+        <v>30</v>
+      </c>
+      <c r="L94">
+        <v>0.91940999999999995</v>
+      </c>
+      <c r="M94">
+        <v>345.75565</v>
+      </c>
+      <c r="N94">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="O94">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="P94">
+        <v>2.3635700000000002</v>
+      </c>
+      <c r="Q94">
+        <v>11.541980000000001</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>49</v>
       </c>
@@ -7704,8 +8602,29 @@
         <f t="shared" si="29"/>
         <v>300.90521775719139</v>
       </c>
-    </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K95">
+        <v>31</v>
+      </c>
+      <c r="L95">
+        <v>0.95167000000000002</v>
+      </c>
+      <c r="M95">
+        <v>355.12054000000001</v>
+      </c>
+      <c r="N95">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="O95">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="P95">
+        <v>2.3635700000000002</v>
+      </c>
+      <c r="Q95">
+        <v>11.541980000000001</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>50</v>
       </c>
@@ -7720,8 +8639,29 @@
         <f t="shared" si="29"/>
         <v>300.89642451052646</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="K96">
+        <v>32</v>
+      </c>
+      <c r="L96">
+        <v>0.98392999999999997</v>
+      </c>
+      <c r="M96">
+        <v>366.38272000000001</v>
+      </c>
+      <c r="N96">
+        <v>2.3248600000000001</v>
+      </c>
+      <c r="O96">
+        <v>1.1624300000000001</v>
+      </c>
+      <c r="P96">
+        <v>3.5259999999999998</v>
+      </c>
+      <c r="Q96">
+        <v>11.542</v>
+      </c>
+    </row>
+    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>51</v>
       </c>
@@ -7736,8 +8676,29 @@
         <f t="shared" si="29"/>
         <v>300.90521775719139</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="K97">
+        <v>33</v>
+      </c>
+      <c r="L97">
+        <v>1.0000599999999999</v>
+      </c>
+      <c r="M97">
+        <v>373.14999</v>
+      </c>
+      <c r="N97">
+        <v>0</v>
+      </c>
+      <c r="O97">
+        <v>0</v>
+      </c>
+      <c r="P97">
+        <v>1</v>
+      </c>
+      <c r="Q97">
+        <v>373.14999</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>52</v>
       </c>
@@ -7753,7 +8714,7 @@
         <v>300.93165380398545</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>53</v>
       </c>
@@ -7769,7 +8730,7 @@
         <v>300.97590193186244</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>54</v>
       </c>
@@ -7785,7 +8746,7 @@
         <v>301.03824547990661</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>55</v>
       </c>
@@ -7801,7 +8762,7 @@
         <v>301.11908365967014</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>56</v>
       </c>
@@ -7817,7 +8778,7 @@
         <v>301.21893411149006</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>57</v>
       </c>
@@ -7833,7 +8794,7 @@
         <v>301.33843621915355</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>58</v>
       </c>
@@ -7849,7 +8810,7 @@
         <v>301.4783552041373</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>59</v>
       </c>
@@ -7865,7 +8826,7 @@
         <v>301.63958702563724</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>60</v>
       </c>
@@ -7881,7 +8842,7 @@
         <v>301.82316411776628</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>61</v>
       </c>
@@ -7897,7 +8858,7 @@
         <v>302.03026200065756</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>62</v>
       </c>
@@ -7913,7 +8874,7 @@
         <v>302.26220680780654</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>63</v>
       </c>
@@ -7929,7 +8890,7 @@
         <v>302.5204837778528</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>64</v>
       </c>
@@ -7945,7 +8906,7 @@
         <v>302.8067467651781</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>65</v>
       </c>
@@ -7961,7 +8922,7 @@
         <v>303.1228288302209</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>66</v>
       </c>
@@ -8545,7 +9506,7 @@
   <dimension ref="B2:O42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8574,7 +9535,7 @@
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5">
         <v>5.0000000000000001E-3</v>
@@ -8598,7 +9559,7 @@
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7">
         <v>280</v>
@@ -8607,22 +9568,22 @@
         <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N7" s="37"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8">
         <v>50000</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N8" s="37"/>
     </row>
@@ -8637,7 +9598,7 @@
         <v>41</v>
       </c>
       <c r="E9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N9" s="37"/>
     </row>
@@ -8676,13 +9637,13 @@
         <v>10</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K12" s="8" t="s">
         <v>12</v>
@@ -8694,7 +9655,7 @@
         <v>11</v>
       </c>
       <c r="N12" s="71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
@@ -8927,7 +9888,7 @@
         <v>8.9990452059999257E-4</v>
       </c>
       <c r="O17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8976,159 +9937,159 @@
         <v>-6.3272190464225006E-3</v>
       </c>
       <c r="O18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="20" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="117" t="s">
-        <v>103</v>
-      </c>
-      <c r="D20" s="118"/>
-      <c r="E20" s="119"/>
+      <c r="C20" s="129" t="s">
+        <v>101</v>
+      </c>
+      <c r="D20" s="130"/>
+      <c r="E20" s="131"/>
     </row>
     <row r="21" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C21" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D21" s="44" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>99</v>
-      </c>
-      <c r="C22" s="124">
+        <v>97</v>
+      </c>
+      <c r="C22" s="112">
         <f>-0.05</f>
         <v>-0.05</v>
       </c>
-      <c r="D22" s="125">
+      <c r="D22" s="113">
         <f t="shared" ref="D22:D31" si="6">-961.538*C22^2-51.851*C22+56.332396</f>
         <v>56.521101000000002</v>
       </c>
-      <c r="E22" s="126">
+      <c r="E22" s="114">
         <f>D22+273.15</f>
         <v>329.67110099999996</v>
       </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C23" s="127">
+      <c r="C23" s="115">
         <f>-0.045</f>
         <v>-4.4999999999999998E-2</v>
       </c>
-      <c r="D23" s="123">
+      <c r="D23" s="111">
         <f t="shared" si="6"/>
         <v>56.718576550000002</v>
       </c>
-      <c r="E23" s="128">
+      <c r="E23" s="116">
         <f t="shared" ref="E23:E42" si="7">D23+273.15</f>
         <v>329.86857655</v>
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C24" s="127">
+      <c r="C24" s="115">
         <v>-0.04</v>
       </c>
-      <c r="D24" s="123">
+      <c r="D24" s="111">
         <f t="shared" si="6"/>
         <v>56.867975200000004</v>
       </c>
-      <c r="E24" s="128">
+      <c r="E24" s="116">
         <f t="shared" si="7"/>
         <v>330.01797519999997</v>
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C25" s="127">
+      <c r="C25" s="115">
         <v>-3.5000000000000003E-2</v>
       </c>
-      <c r="D25" s="123">
+      <c r="D25" s="111">
         <f t="shared" si="6"/>
         <v>56.96929695</v>
       </c>
-      <c r="E25" s="128">
+      <c r="E25" s="116">
         <f t="shared" si="7"/>
         <v>330.11929694999998</v>
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C26" s="127">
+      <c r="C26" s="115">
         <v>-0.03</v>
       </c>
-      <c r="D26" s="123">
+      <c r="D26" s="111">
         <f t="shared" si="6"/>
         <v>57.022541800000006</v>
       </c>
-      <c r="E26" s="128">
+      <c r="E26" s="116">
         <f t="shared" si="7"/>
         <v>330.17254179999998</v>
       </c>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C27" s="127">
+      <c r="C27" s="115">
         <v>-2.5000000000000001E-2</v>
       </c>
-      <c r="D27" s="123">
+      <c r="D27" s="111">
         <f t="shared" si="6"/>
         <v>57.02770975</v>
       </c>
-      <c r="E27" s="128">
+      <c r="E27" s="116">
         <f t="shared" si="7"/>
         <v>330.17770974999996</v>
       </c>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C28" s="127">
+      <c r="C28" s="115">
         <v>-0.02</v>
       </c>
-      <c r="D28" s="123">
+      <c r="D28" s="111">
         <f t="shared" si="6"/>
         <v>56.984800800000002</v>
       </c>
-      <c r="E28" s="128">
+      <c r="E28" s="116">
         <f t="shared" si="7"/>
         <v>330.13480079999999</v>
       </c>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C29" s="127">
+      <c r="C29" s="115">
         <v>-1.4999999999999999E-2</v>
       </c>
-      <c r="D29" s="123">
+      <c r="D29" s="111">
         <f t="shared" si="6"/>
         <v>56.893814949999999</v>
       </c>
-      <c r="E29" s="128">
+      <c r="E29" s="116">
         <f t="shared" si="7"/>
         <v>330.04381494999996</v>
       </c>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C30" s="127">
+      <c r="C30" s="115">
         <v>-0.01</v>
       </c>
-      <c r="D30" s="123">
+      <c r="D30" s="111">
         <f t="shared" si="6"/>
         <v>56.754752200000006</v>
       </c>
-      <c r="E30" s="128">
+      <c r="E30" s="116">
         <f t="shared" si="7"/>
         <v>329.90475219999996</v>
       </c>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C31" s="127">
+      <c r="C31" s="115">
         <v>-5.0000000000000001E-3</v>
       </c>
-      <c r="D31" s="123">
+      <c r="D31" s="111">
         <f t="shared" si="6"/>
         <v>56.56761255</v>
       </c>
-      <c r="E31" s="128">
+      <c r="E31" s="116">
         <f t="shared" si="7"/>
         <v>329.71761254999996</v>
       </c>
@@ -9137,11 +10098,11 @@
       <c r="C32" s="1">
         <v>0</v>
       </c>
-      <c r="D32" s="123">
-        <f>-961.538*C32^2-51.851*C32+56.332396</f>
+      <c r="D32" s="111">
+        <f t="shared" ref="D32:D42" si="8">-961.538*C32^2-51.851*C32+56.332396</f>
         <v>56.332396000000003</v>
       </c>
-      <c r="E32" s="128">
+      <c r="E32" s="116">
         <f t="shared" si="7"/>
         <v>329.48239599999999</v>
       </c>
@@ -9150,11 +10111,11 @@
       <c r="C33" s="1">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="D33" s="123">
-        <f>-961.538*C33^2-51.851*C33+56.332396</f>
+      <c r="D33" s="111">
+        <f t="shared" si="8"/>
         <v>56.049102550000001</v>
       </c>
-      <c r="E33" s="128">
+      <c r="E33" s="116">
         <f t="shared" si="7"/>
         <v>329.19910254999996</v>
       </c>
@@ -9163,11 +10124,11 @@
       <c r="C34" s="1">
         <v>0.01</v>
       </c>
-      <c r="D34" s="123">
-        <f>-961.538*C34^2-51.851*C34+56.332396</f>
+      <c r="D34" s="111">
+        <f t="shared" si="8"/>
         <v>55.7177322</v>
       </c>
-      <c r="E34" s="128">
+      <c r="E34" s="116">
         <f t="shared" si="7"/>
         <v>328.86773219999998</v>
       </c>
@@ -9176,11 +10137,11 @@
       <c r="C35" s="1">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="D35" s="123">
-        <f>-961.538*C35^2-51.851*C35+56.332396</f>
+      <c r="D35" s="111">
+        <f t="shared" si="8"/>
         <v>55.338284950000002</v>
       </c>
-      <c r="E35" s="128">
+      <c r="E35" s="116">
         <f t="shared" si="7"/>
         <v>328.48828494999998</v>
       </c>
@@ -9189,11 +10150,11 @@
       <c r="C36" s="1">
         <v>0.02</v>
       </c>
-      <c r="D36" s="123">
-        <f>-961.538*C36^2-51.851*C36+56.332396</f>
+      <c r="D36" s="111">
+        <f t="shared" si="8"/>
         <v>54.910760800000006</v>
       </c>
-      <c r="E36" s="128">
+      <c r="E36" s="116">
         <f t="shared" si="7"/>
         <v>328.06076079999997</v>
       </c>
@@ -9202,11 +10163,11 @@
       <c r="C37" s="1">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="D37" s="123">
-        <f>-961.538*C37^2-51.851*C37+56.332396</f>
+      <c r="D37" s="111">
+        <f t="shared" si="8"/>
         <v>54.435159750000004</v>
       </c>
-      <c r="E37" s="128">
+      <c r="E37" s="116">
         <f t="shared" si="7"/>
         <v>327.58515975</v>
       </c>
@@ -9215,11 +10176,11 @@
       <c r="C38" s="1">
         <v>0.03</v>
       </c>
-      <c r="D38" s="123">
-        <f>-961.538*C38^2-51.851*C38+56.332396</f>
+      <c r="D38" s="111">
+        <f t="shared" si="8"/>
         <v>53.911481800000004</v>
       </c>
-      <c r="E38" s="128">
+      <c r="E38" s="116">
         <f t="shared" si="7"/>
         <v>327.06148179999997</v>
       </c>
@@ -9228,11 +10189,11 @@
       <c r="C39" s="1">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="D39" s="123">
-        <f>-961.538*C39^2-51.851*C39+56.332396</f>
+      <c r="D39" s="111">
+        <f t="shared" si="8"/>
         <v>53.339726949999999</v>
       </c>
-      <c r="E39" s="128">
+      <c r="E39" s="116">
         <f t="shared" si="7"/>
         <v>326.48972694999998</v>
       </c>
@@ -9241,11 +10202,11 @@
       <c r="C40" s="1">
         <v>0.04</v>
       </c>
-      <c r="D40" s="123">
-        <f>-961.538*C40^2-51.851*C40+56.332396</f>
+      <c r="D40" s="111">
+        <f t="shared" si="8"/>
         <v>52.719895200000003</v>
       </c>
-      <c r="E40" s="128">
+      <c r="E40" s="116">
         <f t="shared" si="7"/>
         <v>325.86989519999997</v>
       </c>
@@ -9254,27 +10215,27 @@
       <c r="C41" s="1">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D41" s="123">
-        <f>-961.538*C41^2-51.851*C41+56.332396</f>
+      <c r="D41" s="111">
+        <f t="shared" si="8"/>
         <v>52.051986550000002</v>
       </c>
-      <c r="E41" s="128">
+      <c r="E41" s="116">
         <f t="shared" si="7"/>
         <v>325.20198654999996</v>
       </c>
     </row>
     <row r="42" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C42" s="3">
         <v>0.05</v>
       </c>
-      <c r="D42" s="129">
-        <f>-961.538*C42^2-51.851*C42+56.332396</f>
+      <c r="D42" s="117">
+        <f t="shared" si="8"/>
         <v>51.336001000000003</v>
       </c>
-      <c r="E42" s="130">
+      <c r="E42" s="118">
         <f t="shared" si="7"/>
         <v>324.48600099999999</v>
       </c>
@@ -9330,15 +10291,15 @@
         <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C5">
         <v>1.2500000000000001E-2</v>
@@ -9361,16 +10322,16 @@
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C6">
         <v>400</v>
       </c>
       <c r="D6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F6">
         <v>430</v>
@@ -9390,12 +10351,12 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -9403,62 +10364,62 @@
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C9">
         <v>273</v>
       </c>
       <c r="D9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="11" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="117" t="s">
-        <v>70</v>
-      </c>
-      <c r="C11" s="118"/>
-      <c r="D11" s="118"/>
-      <c r="E11" s="118"/>
-      <c r="F11" s="118"/>
-      <c r="G11" s="118"/>
-      <c r="H11" s="118"/>
-      <c r="I11" s="119"/>
-      <c r="K11" s="117" t="s">
+      <c r="B11" s="129" t="s">
         <v>68</v>
       </c>
-      <c r="L11" s="118"/>
-      <c r="M11" s="118"/>
-      <c r="N11" s="118"/>
-      <c r="O11" s="118"/>
-      <c r="P11" s="118"/>
-      <c r="Q11" s="118"/>
-      <c r="R11" s="119"/>
+      <c r="C11" s="130"/>
+      <c r="D11" s="130"/>
+      <c r="E11" s="130"/>
+      <c r="F11" s="130"/>
+      <c r="G11" s="130"/>
+      <c r="H11" s="130"/>
+      <c r="I11" s="131"/>
+      <c r="K11" s="129" t="s">
+        <v>66</v>
+      </c>
+      <c r="L11" s="130"/>
+      <c r="M11" s="130"/>
+      <c r="N11" s="130"/>
+      <c r="O11" s="130"/>
+      <c r="P11" s="130"/>
+      <c r="Q11" s="130"/>
+      <c r="R11" s="131"/>
     </row>
     <row r="12" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="120" t="s">
-        <v>71</v>
-      </c>
-      <c r="C12" s="121"/>
-      <c r="D12" s="121"/>
-      <c r="E12" s="121"/>
-      <c r="F12" s="121"/>
-      <c r="G12" s="121"/>
-      <c r="H12" s="122"/>
+      <c r="B12" s="138" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="139"/>
+      <c r="D12" s="139"/>
+      <c r="E12" s="139"/>
+      <c r="F12" s="139"/>
+      <c r="G12" s="139"/>
+      <c r="H12" s="140"/>
       <c r="I12" s="108" t="s">
-        <v>88</v>
-      </c>
-      <c r="K12" s="114" t="s">
-        <v>71</v>
-      </c>
-      <c r="L12" s="115"/>
-      <c r="M12" s="115"/>
-      <c r="N12" s="115"/>
-      <c r="O12" s="115"/>
-      <c r="P12" s="115"/>
-      <c r="Q12" s="116"/>
+        <v>86</v>
+      </c>
+      <c r="K12" s="135" t="s">
+        <v>69</v>
+      </c>
+      <c r="L12" s="136"/>
+      <c r="M12" s="136"/>
+      <c r="N12" s="136"/>
+      <c r="O12" s="136"/>
+      <c r="P12" s="136"/>
+      <c r="Q12" s="137"/>
       <c r="R12" s="108" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -9532,7 +10493,7 @@
         <v>14</v>
       </c>
       <c r="I14" s="105" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J14" s="105"/>
       <c r="K14" s="52">
@@ -9550,16 +10511,16 @@
         <v>0.5</v>
       </c>
       <c r="O14" s="98" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="P14" s="99" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Q14" s="57" t="s">
         <v>14</v>
       </c>
       <c r="R14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.3">
@@ -9588,7 +10549,7 @@
         <v>13.162761400051682</v>
       </c>
       <c r="I15" s="105" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J15" s="105"/>
       <c r="K15" s="53">
@@ -9616,7 +10577,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="R15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.3">
@@ -9646,7 +10607,7 @@
         <v>1.2879995079812421</v>
       </c>
       <c r="I16" s="106" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J16" s="106"/>
       <c r="K16" s="53">
@@ -9675,7 +10636,7 @@
         <v>0.111109733335524</v>
       </c>
       <c r="R16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.3">
@@ -9705,7 +10666,7 @@
         <v>5.4029032398003309E-2</v>
       </c>
       <c r="I17" s="106" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J17" s="106"/>
       <c r="K17" s="53">
@@ -9734,7 +10695,7 @@
         <v>5.8840029405989765E-2</v>
       </c>
       <c r="R17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.3">
@@ -9764,7 +10725,7 @@
         <v>1.190211944354559E-2</v>
       </c>
       <c r="I18" s="106" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J18" s="106"/>
       <c r="K18" s="53">
@@ -9794,7 +10755,7 @@
         <v>3.0349333100625965E-2</v>
       </c>
       <c r="R18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -9824,7 +10785,7 @@
         <v>2.5243706929385388E-3</v>
       </c>
       <c r="I19" s="106" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J19" s="106"/>
       <c r="K19" s="54">
@@ -9853,30 +10814,30 @@
         <v>1.5399887531846505E-2</v>
       </c>
       <c r="R19" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="120" t="s">
-        <v>72</v>
-      </c>
-      <c r="C20" s="121"/>
-      <c r="D20" s="121"/>
-      <c r="E20" s="121"/>
-      <c r="F20" s="121"/>
-      <c r="G20" s="121"/>
-      <c r="H20" s="122"/>
+      <c r="B20" s="138" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="139"/>
+      <c r="D20" s="139"/>
+      <c r="E20" s="139"/>
+      <c r="F20" s="139"/>
+      <c r="G20" s="139"/>
+      <c r="H20" s="140"/>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
-      <c r="K20" s="111" t="s">
-        <v>72</v>
-      </c>
-      <c r="L20" s="112"/>
-      <c r="M20" s="112"/>
-      <c r="N20" s="112"/>
-      <c r="O20" s="112"/>
-      <c r="P20" s="112"/>
-      <c r="Q20" s="113"/>
+      <c r="K20" s="132" t="s">
+        <v>70</v>
+      </c>
+      <c r="L20" s="133"/>
+      <c r="M20" s="133"/>
+      <c r="N20" s="133"/>
+      <c r="O20" s="133"/>
+      <c r="P20" s="133"/>
+      <c r="Q20" s="134"/>
     </row>
     <row r="21" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="93" t="s">
@@ -9949,7 +10910,7 @@
         <v>14</v>
       </c>
       <c r="I22" s="105" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J22" s="105"/>
       <c r="K22" s="52">
@@ -9976,7 +10937,7 @@
         <v>14</v>
       </c>
       <c r="R22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.3">
@@ -10005,7 +10966,7 @@
         <v>0.2587062936209058</v>
       </c>
       <c r="I23" s="106" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J23" s="106"/>
       <c r="K23" s="53">
@@ -10033,7 +10994,7 @@
         <v>6.3464460635133765E-8</v>
       </c>
       <c r="R23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.3">
@@ -10063,7 +11024,7 @@
         <v>0.11377457781579939</v>
       </c>
       <c r="I24" s="106" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J24" s="106"/>
       <c r="K24" s="53">
@@ -10092,7 +11053,7 @@
         <v>-1.8404692430800532E-7</v>
       </c>
       <c r="R24" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.3">
@@ -10122,7 +11083,7 @@
         <v>3.7291454269844843E-2</v>
       </c>
       <c r="I25" s="106" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J25" s="106"/>
       <c r="K25" s="53">
@@ -10151,7 +11112,7 @@
         <v>1.2058248989344544E-7</v>
       </c>
       <c r="R25" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.3">
@@ -10181,7 +11142,7 @@
         <v>1.0242418179336247E-2</v>
       </c>
       <c r="I26" s="106" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J26" s="106"/>
       <c r="K26" s="53">
@@ -10210,7 +11171,7 @@
         <v>1.2058247524057479E-7</v>
       </c>
       <c r="R26" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -10240,7 +11201,7 @@
         <v>2.5411882334526923E-3</v>
       </c>
       <c r="I27" s="106" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J27" s="106"/>
       <c r="K27" s="54">
@@ -10269,30 +11230,30 @@
         <v>3.1315899703087161E-4</v>
       </c>
       <c r="R27" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="120" t="s">
-        <v>73</v>
-      </c>
-      <c r="C28" s="121"/>
-      <c r="D28" s="121"/>
-      <c r="E28" s="121"/>
-      <c r="F28" s="121"/>
-      <c r="G28" s="121"/>
-      <c r="H28" s="122"/>
+      <c r="B28" s="138" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="139"/>
+      <c r="D28" s="139"/>
+      <c r="E28" s="139"/>
+      <c r="F28" s="139"/>
+      <c r="G28" s="139"/>
+      <c r="H28" s="140"/>
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
-      <c r="K28" s="111" t="s">
-        <v>73</v>
-      </c>
-      <c r="L28" s="112"/>
-      <c r="M28" s="112"/>
-      <c r="N28" s="112"/>
-      <c r="O28" s="112"/>
-      <c r="P28" s="112"/>
-      <c r="Q28" s="113"/>
+      <c r="K28" s="132" t="s">
+        <v>71</v>
+      </c>
+      <c r="L28" s="133"/>
+      <c r="M28" s="133"/>
+      <c r="N28" s="133"/>
+      <c r="O28" s="133"/>
+      <c r="P28" s="133"/>
+      <c r="Q28" s="134"/>
     </row>
     <row r="29" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="93" t="s">
@@ -10365,7 +11326,7 @@
         <v>14</v>
       </c>
       <c r="I30" s="105" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J30" s="105"/>
       <c r="K30" s="52">
@@ -10392,7 +11353,7 @@
         <v>14</v>
       </c>
       <c r="R30" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.3">
@@ -10421,7 +11382,7 @@
         <v>0.2587049245535939</v>
       </c>
       <c r="I31" s="106" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J31" s="106"/>
       <c r="K31" s="53">
@@ -10449,7 +11410,7 @@
         <v>0.99357636919766734</v>
       </c>
       <c r="R31" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.3">
@@ -10479,7 +11440,7 @@
         <v>0.11377597779970303</v>
       </c>
       <c r="I32" s="106" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J32" s="106"/>
       <c r="K32" s="53">
@@ -10508,7 +11469,7 @@
         <v>0.97510368613467613</v>
       </c>
       <c r="R32" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="2:18" ht="28.8" x14ac:dyDescent="0.3">
@@ -10538,7 +11499,7 @@
         <v>3.7290647018494237E-2</v>
       </c>
       <c r="I33" s="107" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J33" s="107"/>
       <c r="K33" s="53">
@@ -10567,7 +11528,7 @@
         <v>0.91101063062196352</v>
       </c>
       <c r="R33" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.3">
@@ -10597,7 +11558,7 @@
         <v>1.0255229178946891E-2</v>
       </c>
       <c r="I34" s="106" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J34" s="106"/>
       <c r="K34" s="53">
@@ -10626,7 +11587,7 @@
         <v>0.74420427238555509</v>
       </c>
       <c r="R34" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="2:18" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -10656,7 +11617,7 @@
         <v>2.5221367373014216E-3</v>
       </c>
       <c r="I35" s="107" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J35" s="107"/>
       <c r="K35" s="54">
@@ -10685,7 +11646,7 @@
         <v>0.48149343845078624</v>
       </c>
       <c r="R35" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -10714,7 +11675,7 @@
         <v>0.1681868824703702</v>
       </c>
       <c r="R36" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -10738,8 +11699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K11" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20:Q20"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10775,15 +11736,15 @@
         <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C5">
         <v>1.2500000000000001E-2</v>
@@ -10806,16 +11767,16 @@
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C6">
         <v>400</v>
       </c>
       <c r="D6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F6">
         <v>430</v>
@@ -10835,12 +11796,12 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -10848,62 +11809,62 @@
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="11" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="117" t="s">
-        <v>70</v>
-      </c>
-      <c r="C11" s="118"/>
-      <c r="D11" s="118"/>
-      <c r="E11" s="118"/>
-      <c r="F11" s="118"/>
-      <c r="G11" s="118"/>
-      <c r="H11" s="118"/>
-      <c r="I11" s="119"/>
-      <c r="K11" s="117" t="s">
+      <c r="B11" s="129" t="s">
         <v>68</v>
       </c>
-      <c r="L11" s="118"/>
-      <c r="M11" s="118"/>
-      <c r="N11" s="118"/>
-      <c r="O11" s="118"/>
-      <c r="P11" s="118"/>
-      <c r="Q11" s="118"/>
-      <c r="R11" s="119"/>
+      <c r="C11" s="130"/>
+      <c r="D11" s="130"/>
+      <c r="E11" s="130"/>
+      <c r="F11" s="130"/>
+      <c r="G11" s="130"/>
+      <c r="H11" s="130"/>
+      <c r="I11" s="131"/>
+      <c r="K11" s="129" t="s">
+        <v>66</v>
+      </c>
+      <c r="L11" s="130"/>
+      <c r="M11" s="130"/>
+      <c r="N11" s="130"/>
+      <c r="O11" s="130"/>
+      <c r="P11" s="130"/>
+      <c r="Q11" s="130"/>
+      <c r="R11" s="131"/>
     </row>
     <row r="12" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="120" t="s">
-        <v>71</v>
-      </c>
-      <c r="C12" s="121"/>
-      <c r="D12" s="121"/>
-      <c r="E12" s="121"/>
-      <c r="F12" s="121"/>
-      <c r="G12" s="121"/>
-      <c r="H12" s="122"/>
+      <c r="B12" s="138" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="139"/>
+      <c r="D12" s="139"/>
+      <c r="E12" s="139"/>
+      <c r="F12" s="139"/>
+      <c r="G12" s="139"/>
+      <c r="H12" s="140"/>
       <c r="I12" s="108" t="s">
-        <v>88</v>
-      </c>
-      <c r="K12" s="114" t="s">
-        <v>71</v>
-      </c>
-      <c r="L12" s="115"/>
-      <c r="M12" s="115"/>
-      <c r="N12" s="115"/>
-      <c r="O12" s="115"/>
-      <c r="P12" s="115"/>
-      <c r="Q12" s="116"/>
+        <v>86</v>
+      </c>
+      <c r="K12" s="135" t="s">
+        <v>69</v>
+      </c>
+      <c r="L12" s="136"/>
+      <c r="M12" s="136"/>
+      <c r="N12" s="136"/>
+      <c r="O12" s="136"/>
+      <c r="P12" s="136"/>
+      <c r="Q12" s="137"/>
       <c r="R12" s="108" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -10977,7 +11938,7 @@
         <v>14</v>
       </c>
       <c r="I14" s="105" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J14" s="105"/>
       <c r="K14" s="52">
@@ -10995,16 +11956,16 @@
         <v>0.5</v>
       </c>
       <c r="O14" s="98" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="P14" s="99" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Q14" s="57" t="s">
         <v>14</v>
       </c>
       <c r="R14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.3">
@@ -11033,7 +11994,7 @@
         <v>0.21123781245720175</v>
       </c>
       <c r="I15" s="105" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J15" s="105"/>
       <c r="K15" s="53">
@@ -11061,7 +12022,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="R15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.3">
@@ -11091,7 +12052,7 @@
         <v>9.8802888521172555E-2</v>
       </c>
       <c r="I16" s="105" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J16" s="106"/>
       <c r="K16" s="53">
@@ -11120,7 +12081,7 @@
         <v>0.111109733335524</v>
       </c>
       <c r="R16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.3">
@@ -11150,7 +12111,7 @@
         <v>3.3587025425345085E-2</v>
       </c>
       <c r="I17" s="105" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J17" s="106"/>
       <c r="K17" s="53">
@@ -11179,7 +12140,7 @@
         <v>5.8840029405989765E-2</v>
       </c>
       <c r="R17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.3">
@@ -11209,7 +12170,7 @@
         <v>9.3886497686890384E-3</v>
       </c>
       <c r="I18" s="106" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="J18" s="106"/>
       <c r="K18" s="53">
@@ -11239,7 +12200,7 @@
         <v>3.0349333100625965E-2</v>
       </c>
       <c r="R18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -11269,7 +12230,7 @@
         <v>2.3594935596523764E-3</v>
       </c>
       <c r="I19" s="106" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="J19" s="106"/>
       <c r="K19" s="54">
@@ -11298,30 +12259,30 @@
         <v>1.5399887531846505E-2</v>
       </c>
       <c r="R19" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="120" t="s">
-        <v>72</v>
-      </c>
-      <c r="C20" s="121"/>
-      <c r="D20" s="121"/>
-      <c r="E20" s="121"/>
-      <c r="F20" s="121"/>
-      <c r="G20" s="121"/>
-      <c r="H20" s="122"/>
+      <c r="B20" s="138" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="139"/>
+      <c r="D20" s="139"/>
+      <c r="E20" s="139"/>
+      <c r="F20" s="139"/>
+      <c r="G20" s="139"/>
+      <c r="H20" s="140"/>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
-      <c r="K20" s="111" t="s">
-        <v>72</v>
-      </c>
-      <c r="L20" s="112"/>
-      <c r="M20" s="112"/>
-      <c r="N20" s="112"/>
-      <c r="O20" s="112"/>
-      <c r="P20" s="112"/>
-      <c r="Q20" s="113"/>
+      <c r="K20" s="132" t="s">
+        <v>70</v>
+      </c>
+      <c r="L20" s="133"/>
+      <c r="M20" s="133"/>
+      <c r="N20" s="133"/>
+      <c r="O20" s="133"/>
+      <c r="P20" s="133"/>
+      <c r="Q20" s="134"/>
     </row>
     <row r="21" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="93" t="s">
@@ -11394,7 +12355,7 @@
         <v>14</v>
       </c>
       <c r="I22" s="105" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="J22" s="105"/>
       <c r="K22" s="52">
@@ -11421,7 +12382,7 @@
         <v>14</v>
       </c>
       <c r="R22" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.3">
@@ -11450,7 +12411,7 @@
         <v>0.21123761188390039</v>
       </c>
       <c r="I23" s="105" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="J23" s="106"/>
       <c r="K23" s="53">
@@ -11478,7 +12439,7 @@
         <v>5.4013764858511942E-4</v>
       </c>
       <c r="R23" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.3">
@@ -11508,7 +12469,7 @@
         <v>9.8802273306240349E-2</v>
       </c>
       <c r="I24" s="106" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J24" s="106"/>
       <c r="K24" s="53">
@@ -11537,7 +12498,7 @@
         <v>1.0324071136936829E-2</v>
       </c>
       <c r="R24" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.3">
@@ -11567,7 +12528,7 @@
         <v>3.3586356639078205E-2</v>
       </c>
       <c r="I25" s="106" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J25" s="106"/>
       <c r="K25" s="53">
@@ -11596,7 +12557,7 @@
         <v>0.20540332647774823</v>
       </c>
       <c r="R25" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.3">
@@ -11626,7 +12587,7 @@
         <v>9.3922249301873588E-3</v>
       </c>
       <c r="I26" s="106" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J26" s="106"/>
       <c r="K26" s="53">
@@ -11655,7 +12616,7 @@
         <v>2.4807785930343353</v>
       </c>
       <c r="R26" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -11685,7 +12646,7 @@
         <v>2.3617037413172538E-3</v>
       </c>
       <c r="I27" s="106" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J27" s="106"/>
       <c r="K27" s="54">
@@ -11714,30 +12675,30 @@
         <v>2.8442702972673031</v>
       </c>
       <c r="R27" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="120" t="s">
-        <v>73</v>
-      </c>
-      <c r="C28" s="121"/>
-      <c r="D28" s="121"/>
-      <c r="E28" s="121"/>
-      <c r="F28" s="121"/>
-      <c r="G28" s="121"/>
-      <c r="H28" s="122"/>
+      <c r="B28" s="138" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="139"/>
+      <c r="D28" s="139"/>
+      <c r="E28" s="139"/>
+      <c r="F28" s="139"/>
+      <c r="G28" s="139"/>
+      <c r="H28" s="140"/>
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
-      <c r="K28" s="111" t="s">
-        <v>73</v>
-      </c>
-      <c r="L28" s="112"/>
-      <c r="M28" s="112"/>
-      <c r="N28" s="112"/>
-      <c r="O28" s="112"/>
-      <c r="P28" s="112"/>
-      <c r="Q28" s="113"/>
+      <c r="K28" s="132" t="s">
+        <v>71</v>
+      </c>
+      <c r="L28" s="133"/>
+      <c r="M28" s="133"/>
+      <c r="N28" s="133"/>
+      <c r="O28" s="133"/>
+      <c r="P28" s="133"/>
+      <c r="Q28" s="134"/>
     </row>
     <row r="29" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="93" t="s">
@@ -11810,7 +12771,7 @@
         <v>14</v>
       </c>
       <c r="I30" s="105" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J30" s="105"/>
       <c r="K30" s="52">
@@ -11837,7 +12798,7 @@
         <v>14</v>
       </c>
       <c r="R30" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.3">
@@ -11866,7 +12827,7 @@
         <v>0.21123812615472437</v>
       </c>
       <c r="I31" s="106" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J31" s="106"/>
       <c r="K31" s="53">
@@ -11894,7 +12855,7 @@
         <v>0.83330481421532032</v>
       </c>
       <c r="R31" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.3">
@@ -11924,7 +12885,7 @@
         <v>9.8801897751054274E-2</v>
       </c>
       <c r="I32" s="106" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J32" s="106"/>
       <c r="K32" s="53">
@@ -11953,7 +12914,7 @@
         <v>0.76344909888372448</v>
       </c>
       <c r="R32" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.3">
@@ -11983,7 +12944,7 @@
         <v>3.3589977954342834E-2</v>
       </c>
       <c r="I33" s="106" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J33" s="107"/>
       <c r="K33" s="53">
@@ -12012,7 +12973,7 @@
         <v>0.66322086690443416</v>
       </c>
       <c r="R33" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.3">
@@ -12042,7 +13003,7 @@
         <v>9.3909819093312731E-3</v>
       </c>
       <c r="I34" s="106" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="J34" s="106"/>
       <c r="K34" s="53">
@@ -12071,7 +13032,7 @@
         <v>0.52629789365696655</v>
       </c>
       <c r="R34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="35" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -12101,7 +13062,7 @@
         <v>2.3640364572853484E-3</v>
       </c>
       <c r="I35" s="107" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J35" s="107"/>
       <c r="K35" s="54">
@@ -12130,7 +13091,7 @@
         <v>0.3571840042714553</v>
       </c>
       <c r="R35" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -12144,7 +13105,7 @@
         <f>L36-1</f>
         <v>100</v>
       </c>
-      <c r="N36" s="140">
+      <c r="N36" s="128">
         <f t="shared" si="13"/>
         <v>0.01</v>
       </c>
@@ -12159,7 +13120,7 @@
         <v>0.13462780102357103</v>
       </c>
       <c r="R36" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="37" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -12173,7 +13134,7 @@
         <f>L37-1</f>
         <v>114</v>
       </c>
-      <c r="N37" s="140">
+      <c r="N37" s="128">
         <f t="shared" si="13"/>
         <v>8.771929824561403E-3</v>
       </c>
@@ -12188,7 +13149,7 @@
         <v>2.752057601259009E-2</v>
       </c>
       <c r="R37" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>